<commit_message>
tab pertumbuhan ekonomi done
</commit_message>
<xml_diff>
--- a/data/data_pdrb.xlsx
+++ b/data/data_pdrb.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cf16fee0dbbc24c2/Work/Training/BPS Orientation/PDRB/gdp-dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="11_F25DC773A252ABDACC10484CF9997BDA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC187E34-5AA8-44D2-A897-65C32E25FFD3}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="11_F25DC773A252ABDACC10484CF9997BDA5BDE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF5A659A-9C31-4631-9C1D-32A6A5156C35}"/>
   <bookViews>
-    <workbookView xWindow="2328" yWindow="2412" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="adhb" sheetId="1" r:id="rId1"/>
@@ -7946,8 +7946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3836C6D9-8DD9-4EF1-A3F0-E1606414A771}">
   <dimension ref="A1:AI66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15023,11 +15023,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37A52856-D961-4F40-97BB-D2B9EADD390D}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.88671875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">

</xml_diff>